<commit_message>
Update to ID on metasheet
</commit_message>
<xml_diff>
--- a/VQC R work/Albuwell Data Sheets/Long_PFAS_Metadata.xlsx
+++ b/VQC R work/Albuwell Data Sheets/Long_PFAS_Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victoriaqc/Documents/GitHub/PFAS_met_cage/VQC R work/Albuwell Data Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DA6DDA-7BBB-F045-AAC8-BA6D17AC6C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF26A6A-2AE5-4848-8C98-D540CEF6F040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3340" yWindow="6200" windowWidth="25320" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6:AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -983,79 +983,79 @@
         <v>0</v>
       </c>
       <c r="B6" s="1">
-        <v>20</v>
+        <v>3920</v>
       </c>
       <c r="C6" s="1">
-        <v>21</v>
+        <v>3921</v>
       </c>
       <c r="D6" s="1">
-        <v>22</v>
+        <v>3922</v>
       </c>
       <c r="E6" s="1">
-        <v>23</v>
+        <v>3923</v>
       </c>
       <c r="F6" s="1">
-        <v>32</v>
+        <v>3932</v>
       </c>
       <c r="G6" s="1">
-        <v>33</v>
+        <v>3933</v>
       </c>
       <c r="H6" s="1">
-        <v>34</v>
+        <v>3934</v>
       </c>
       <c r="I6" s="1">
-        <v>35</v>
+        <v>3935</v>
       </c>
       <c r="J6" s="1">
-        <v>36</v>
+        <v>3936</v>
       </c>
       <c r="K6" s="1">
-        <v>37</v>
+        <v>3937</v>
       </c>
       <c r="L6" s="1">
-        <v>38</v>
+        <v>3938</v>
       </c>
       <c r="M6" s="1">
-        <v>39</v>
+        <v>3939</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1">
-        <v>20</v>
+        <v>3920</v>
       </c>
       <c r="R6" s="1">
-        <v>21</v>
+        <v>3921</v>
       </c>
       <c r="S6" s="1">
-        <v>22</v>
+        <v>3922</v>
       </c>
       <c r="T6" s="1">
-        <v>23</v>
+        <v>3923</v>
       </c>
       <c r="U6" s="1">
-        <v>32</v>
+        <v>3932</v>
       </c>
       <c r="V6" s="1">
-        <v>33</v>
+        <v>3933</v>
       </c>
       <c r="W6" s="1">
-        <v>34</v>
+        <v>3934</v>
       </c>
       <c r="X6" s="1">
-        <v>35</v>
+        <v>3935</v>
       </c>
       <c r="Y6" s="1">
-        <v>36</v>
+        <v>3936</v>
       </c>
       <c r="Z6" s="1">
-        <v>37</v>
+        <v>3937</v>
       </c>
       <c r="AA6" s="1">
-        <v>38</v>
+        <v>3938</v>
       </c>
       <c r="AB6" s="1">
-        <v>39</v>
+        <v>3939</v>
       </c>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>

</xml_diff>

<commit_message>
update to PFAS experiment.
</commit_message>
<xml_diff>
--- a/VQC R work/Albuwell Data Sheets/Long_PFAS_Metadata.xlsx
+++ b/VQC R work/Albuwell Data Sheets/Long_PFAS_Metadata.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="159" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A103D56-228A-4813-B4F2-F760FE6C2C5A}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\OneDrive - University of Southern California\Github\PFAS_met_cage\VQC R work\Albuwell Data Sheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD05EB1-7BA8-4E3F-83F8-DA47D4A05535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,78 +41,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>20 Base</t>
-  </si>
-  <si>
-    <t>21 Base</t>
-  </si>
-  <si>
-    <t>22 Base</t>
-  </si>
-  <si>
-    <t>23 Base</t>
-  </si>
-  <si>
-    <t>32 Base</t>
-  </si>
-  <si>
-    <t>33 Base</t>
-  </si>
-  <si>
-    <t>34 Base</t>
-  </si>
-  <si>
-    <t>35 Base</t>
-  </si>
-  <si>
-    <t>36 Base</t>
-  </si>
-  <si>
-    <t>37 Base</t>
-  </si>
-  <si>
-    <t>38 Base</t>
-  </si>
-  <si>
-    <t>39 Base</t>
-  </si>
-  <si>
-    <t>20 Final</t>
-  </si>
-  <si>
-    <t>21 Final</t>
-  </si>
-  <si>
-    <t>22 Final</t>
-  </si>
-  <si>
-    <t>23 Final</t>
-  </si>
-  <si>
-    <t>32 Final</t>
-  </si>
-  <si>
-    <t>33 Final</t>
-  </si>
-  <si>
-    <t>34 Final</t>
-  </si>
-  <si>
-    <t>35 Final</t>
-  </si>
-  <si>
-    <t>36 Final</t>
-  </si>
-  <si>
-    <t>37 Final</t>
-  </si>
-  <si>
-    <t>38 Final</t>
-  </si>
-  <si>
-    <t>39 Final</t>
-  </si>
-  <si>
     <t>Treatment</t>
   </si>
   <si>
@@ -157,13 +90,85 @@
   </si>
   <si>
     <t>ID_2</t>
+  </si>
+  <si>
+    <t>3920_Base</t>
+  </si>
+  <si>
+    <t>3921_Base</t>
+  </si>
+  <si>
+    <t>3922_Base</t>
+  </si>
+  <si>
+    <t>3923_Base</t>
+  </si>
+  <si>
+    <t>3932_Base</t>
+  </si>
+  <si>
+    <t>3933_Base</t>
+  </si>
+  <si>
+    <t>3934_Base</t>
+  </si>
+  <si>
+    <t>3935_Base</t>
+  </si>
+  <si>
+    <t>3936_Base</t>
+  </si>
+  <si>
+    <t>3937_Base</t>
+  </si>
+  <si>
+    <t>3938_Base</t>
+  </si>
+  <si>
+    <t>3939_Base</t>
+  </si>
+  <si>
+    <t>3920_ Final</t>
+  </si>
+  <si>
+    <t>3921_Final</t>
+  </si>
+  <si>
+    <t>3922_Final</t>
+  </si>
+  <si>
+    <t>3923_Final</t>
+  </si>
+  <si>
+    <t>3932_Final</t>
+  </si>
+  <si>
+    <t>3933_Final</t>
+  </si>
+  <si>
+    <t>3934_Final</t>
+  </si>
+  <si>
+    <t>3935_Final</t>
+  </si>
+  <si>
+    <t>3936_Final</t>
+  </si>
+  <si>
+    <t>3937_Final</t>
+  </si>
+  <si>
+    <t>3938_Final</t>
+  </si>
+  <si>
+    <t>3939_Final</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,11 +543,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AB5" sqref="AB5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -554,173 +559,173 @@
     <col min="25" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>2.75</v>
@@ -798,175 +803,175 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1">
         <v>20</v>

</xml_diff>